<commit_message>
2019 added missing coordinates and combined 2014 to 2020 cameras and locations
</commit_message>
<xml_diff>
--- a/2019/Cameras_2019_work.xlsx
+++ b/2019/Cameras_2019_work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elise/Desktop/MP/Belize-MP-Bruno-Boos/2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111F24F0-68B3-194C-B8E3-5132D3B2A757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F11C288-5DD6-C347-AD11-F183BCAAF919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16000" xr2:uid="{3D9382E5-193C-6B48-BF0E-C219740D5475}"/>
   </bookViews>
@@ -309,7 +309,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -330,6 +330,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -358,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -367,6 +373,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,7 +692,7 @@
   <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2088,7 +2096,12 @@
       <c r="H37">
         <v>50</v>
       </c>
-      <c r="I37" s="5"/>
+      <c r="I37" s="8">
+        <v>286486</v>
+      </c>
+      <c r="J37" s="9">
+        <v>1954650</v>
+      </c>
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
     </row>

</xml_diff>